<commit_message>
edits to the ground truth file
</commit_message>
<xml_diff>
--- a/Ground_Truth_Data_Competition_Files.xlsx
+++ b/Ground_Truth_Data_Competition_Files.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caterpillar-my.sharepoint.com/personal/cline_kyle_j_cat_com/Documents/Machine Data Insights/UIUC Key Account Manager/HackIllinois 2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccoydj2\Desktop\HackIllinois\2020_Challenge_IOT_Analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DC3BDC7-AA1B-474F-B5E8-4A3AC38F4A9C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B084490-132B-4E5C-8CA1-4F17A820E186}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{370DDFDF-EEBF-427C-816B-663081CF2FA6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{370DDFDF-EEBF-427C-816B-663081CF2FA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,7 +73,7 @@
     <t>Channel flatlined to 0 for the entire day (0 deg C in early July)</t>
   </si>
   <si>
-    <t>Channel recorded constant 63 for the entire day</t>
+    <t>Channel recorded constant for the entire day but should not have</t>
   </si>
 </sst>
 </file>
@@ -429,19 +429,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF7F704-0824-4E51-93EC-00A205472A75}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
-    <col min="6" max="6" width="65.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.08984375" customWidth="1"/>
+    <col min="6" max="6" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +459,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>40732</v>
       </c>
@@ -479,7 +477,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>40731</v>
       </c>
@@ -497,7 +495,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>40733</v>
       </c>
@@ -515,7 +513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>40659</v>
       </c>
@@ -533,7 +531,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>40725</v>
       </c>
@@ -553,7 +551,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>40322</v>
       </c>
@@ -573,7 +571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>40324</v>
       </c>
@@ -593,7 +591,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>40325</v>
       </c>
@@ -613,7 +611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>40737</v>
       </c>
@@ -633,7 +631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>40761</v>
       </c>
@@ -653,7 +651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>40760</v>
       </c>
@@ -673,7 +671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>40772</v>
       </c>
@@ -693,7 +691,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>40762</v>
       </c>
@@ -713,7 +711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>40767</v>
       </c>
@@ -733,7 +731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>40764</v>
       </c>
@@ -753,7 +751,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>40736</v>
       </c>
@@ -773,7 +771,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>40785</v>
       </c>
@@ -793,7 +791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>40708</v>
       </c>
@@ -813,7 +811,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>40400</v>
       </c>
@@ -833,7 +831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>40401</v>
       </c>
@@ -853,7 +851,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>40405</v>
       </c>
@@ -873,7 +871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>44057</v>
       </c>
@@ -893,7 +891,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>40341</v>
       </c>
@@ -913,7 +911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>40335</v>
       </c>
@@ -933,7 +931,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>40342</v>
       </c>
@@ -953,16 +951,16 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B30" s="2"/>
     </row>
   </sheetData>
@@ -980,7 +978,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1214,18 +1212,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1248,14 +1246,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF3C1349-D093-46B5-AD72-D63A1AAC6AAF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA210480-C007-4E7E-9535-5B37249840F5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1270,4 +1260,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF3C1349-D093-46B5-AD72-D63A1AAC6AAF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>